<commit_message>
Remove unused code, change viewmodels to wrapper of interfaces, add custom property realname to cells. remove msexcel2003 nuget pack ref
</commit_message>
<xml_diff>
--- a/Medidata.Cloud.Tsdv.Loader.Tests/TestHelpers/tsdv_test.xlsx
+++ b/Medidata.Cloud.Tsdv.Loader.Tests/TestHelpers/tsdv_test.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Block Plans" sheetId="1" r:id="R3b5ac3a1ad3248d2"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BlockPlans" sheetId="1" r:id="Ref1732d220294a46"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -11,38 +11,38 @@
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetData>
     <x:row>
-      <x:c t="str">
-        <x:v>Block Plan Name</x:v>
+      <x:c xmlns:p4="mdsol" t="str" p4:RealName="Name">
+        <x:v>Name</x:v>
       </x:c>
-      <x:c t="str">
-        <x:v>Block Plan Type</x:v>
+      <x:c xmlns:p4="mdsol" t="str" p4:RealName="BlockPlanType">
+        <x:v>BlockPlanType</x:v>
       </x:c>
-      <x:c t="str">
-        <x:v>Study/SiteGroup/SiteName</x:v>
+      <x:c xmlns:p4="mdsol" t="str" p4:RealName="ObjectName">
+        <x:v>ObjectName</x:v>
       </x:c>
-      <x:c t="str">
-        <x:v>Contains Subjects</x:v>
+      <x:c xmlns:p4="mdsol" t="str" p4:RealName="IsProdInUse">
+        <x:v>IsProdInUse</x:v>
       </x:c>
-      <x:c t="str">
-        <x:v>Data Entry Role</x:v>
+      <x:c xmlns:p4="mdsol" t="str" p4:RealName="RoleName">
+        <x:v>RoleName</x:v>
       </x:c>
-      <x:c t="str">
-        <x:v>Block Plan Status</x:v>
+      <x:c xmlns:p4="mdsol" t="str" p4:RealName="Activated">
+        <x:v>Activated</x:v>
       </x:c>
-      <x:c t="str">
-        <x:v>Plan Activated By</x:v>
+      <x:c xmlns:p4="mdsol" t="str" p4:RealName="ActivatedUserName">
+        <x:v>ActivatedUserName</x:v>
       </x:c>
-      <x:c t="str">
-        <x:v>Average Subjects/Site</x:v>
+      <x:c xmlns:p4="mdsol" t="str" p4:RealName="AverageSubjectPerSite">
+        <x:v>AverageSubjectPerSite</x:v>
       </x:c>
-      <x:c t="str">
-        <x:v>Estimated Coverage</x:v>
+      <x:c xmlns:p4="mdsol" t="str" p4:RealName="CoveragePercent">
+        <x:v>CoveragePercent</x:v>
       </x:c>
-      <x:c t="str">
-        <x:v>Using Matrix</x:v>
+      <x:c xmlns:p4="mdsol" t="str" p4:RealName="MatrixName">
+        <x:v>MatrixName</x:v>
       </x:c>
-      <x:c t="str">
-        <x:v>Estimated Date</x:v>
+      <x:c xmlns:p4="mdsol" t="str" p4:RealName="DateEstimated">
+        <x:v>DateEstimated</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -56,13 +56,13 @@
         <x:v>ObjectName1</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>Yes</x:v>
+        <x:v>True</x:v>
       </x:c>
       <x:c t="str">
         <x:v>Role 1</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>Active</x:v>
+        <x:v>True</x:v>
       </x:c>
       <x:c t="str">
         <x:v>cheng</x:v>
@@ -77,7 +77,7 @@
         <x:v>DefaultMatrix</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>11/15/2015 9:54:38 PM</x:v>
+        <x:v>11/16/2015 10:08:31 PM</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>